<commit_message>
Verity as source for method 2 IFR when higher than Ferguson
</commit_message>
<xml_diff>
--- a/IC-capaciteit.xlsx
+++ b/IC-capaciteit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="7720" windowWidth="25600" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COVID.calc.groepsimmuniteit (3)" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="142">
   <si>
     <t>=</t>
   </si>
@@ -324,18 +324,12 @@
     <t>IC-patienten</t>
   </si>
   <si>
-    <t>95%CI low</t>
-  </si>
-  <si>
     <t>95%CI high</t>
   </si>
   <si>
     <t>age group</t>
   </si>
   <si>
-    <t>sum = infected</t>
-  </si>
-  <si>
     <t>error bar low</t>
   </si>
   <si>
@@ -345,21 +339,12 @@
     <t>95% CI middle</t>
   </si>
   <si>
-    <t>Figure 3 C in Verity et al. (Imp. College)</t>
-  </si>
-  <si>
-    <t>Table 1 in Ferguson et al. (Imp. College)</t>
-  </si>
-  <si>
     <t>besmettingen</t>
   </si>
   <si>
     <t>inwoners NL</t>
   </si>
   <si>
-    <t>CAF</t>
-  </si>
-  <si>
     <t>ZKH-opnames</t>
   </si>
   <si>
@@ -441,9 +426,6 @@
     <t>inwoners totaal</t>
   </si>
   <si>
-    <t>CAF, opname- en IC-kansen:</t>
-  </si>
-  <si>
     <t>https://nos.nl/artikel/2327537-171-coronapatienten-op-de-intensive-care-ziekenhuizen-stralen-rust-uit.html</t>
   </si>
   <si>
@@ -469,6 +451,45 @@
   </si>
   <si>
     <t>ascertainment rate in studie IC load</t>
+  </si>
+  <si>
+    <t>Figure 3 C in Verity et al. (Imperial College)</t>
+  </si>
+  <si>
+    <t>Table 1 in Ferguson et al. (Imperial College)</t>
+  </si>
+  <si>
+    <t>Alternatieve bronnen</t>
+  </si>
+  <si>
+    <t>https://www.researchsquare.com/article/rs-17453/v1</t>
+  </si>
+  <si>
+    <t>sCFR was 0.5% (0.1%-1.3%), 0.5% (0.2%-1.1%) and 2.7% (1.5%-4.7%) for those aged 15-44, 45-64 and &gt;64 years</t>
+  </si>
+  <si>
+    <t>Wu et al. Estimating clinical severity of COVID-19 from the transmission dynamics in Wuhan, China</t>
+  </si>
+  <si>
+    <t>Imperial College</t>
+  </si>
+  <si>
+    <t>Diamond Princess</t>
+  </si>
+  <si>
+    <t>CAF's, IFR voor 0-19j:</t>
+  </si>
+  <si>
+    <t>IFR's 20j+, opname- en IC-kansen:</t>
+  </si>
+  <si>
+    <t>CAF = symptomatic / infected</t>
+  </si>
+  <si>
+    <t>infected = sum</t>
+  </si>
+  <si>
+    <t>95%CI low (Clopper Pearson method)</t>
   </si>
 </sst>
 </file>
@@ -481,7 +502,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,6 +604,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue Light"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue Light"/>
     </font>
@@ -742,7 +769,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -866,8 +893,45 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1068,14 +1132,22 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="160">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1197,6 +1269,43 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1298,8 +1407,114 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Imperial College</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40-49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50-59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60-69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70-79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Diamond Princess'!$U$5:$U$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.0836550836550836</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.133204633204633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.521879021879022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9002574002574</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.858429858429858</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48970398970399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.406048906048906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.167953667953668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diamond Princess</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1310,7 +1525,7 @@
             <c:noEndCap val="1"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Diamond Princess'!$I$5:$I$13</c:f>
+                <c:f>'Diamond Princess'!$I$7:$I$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
@@ -1346,7 +1561,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Diamond Princess'!$H$5:$H$13</c:f>
+                <c:f>'Diamond Princess'!$H$7:$H$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="9"/>
@@ -1383,7 +1598,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Diamond Princess'!$A$5:$A$13</c:f>
+              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1418,7 +1633,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Diamond Princess'!$E$5:$E$13</c:f>
+              <c:f>'Diamond Princess'!$E$7:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1456,10 +1671,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Diamond Princess'!$J$4</c:f>
+              <c:f>'Diamond Princess'!$J$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1470,41 +1685,52 @@
           </c:tx>
           <c:spPr>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:intercept val="0.0"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.059249343832021"/>
-                  <c:y val="-0.383882327209099"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr algn="r">
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40-49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50-59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60-69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70-79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Diamond Princess'!$J$5:$J$13</c:f>
+              <c:f>'Diamond Princess'!$J$7:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1550,11 +1776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2064230632"/>
-        <c:axId val="2069771000"/>
+        <c:axId val="2117780200"/>
+        <c:axId val="2117783400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2064230632"/>
+        <c:axId val="2117780200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1563,7 +1789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069771000"/>
+        <c:crossAx val="2117783400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +1797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069771000"/>
+        <c:axId val="2117783400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,11 +1823,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064230632"/>
+        <c:crossAx val="2117780200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1627,16 +1853,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2623,7 +2849,7 @@
         <f t="shared" si="1"/>
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G39" s="126" t="s">
+      <c r="G39" s="128" t="s">
         <v>73</v>
       </c>
       <c r="H39" s="14" t="s">
@@ -2700,7 +2926,7 @@
         <f t="shared" si="1"/>
         <v>1.5E-3</v>
       </c>
-      <c r="G40" s="126"/>
+      <c r="G40" s="128"/>
       <c r="H40" s="14" t="s">
         <v>7</v>
       </c>
@@ -2775,7 +3001,7 @@
         <f t="shared" si="1"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G41" s="126"/>
+      <c r="G41" s="128"/>
       <c r="H41" s="14" t="s">
         <v>6</v>
       </c>
@@ -3218,7 +3444,7 @@
       </c>
     </row>
     <row r="53" spans="2:12" ht="17" customHeight="1">
-      <c r="G53" s="127" t="s">
+      <c r="G53" s="129" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -3240,7 +3466,7 @@
       </c>
     </row>
     <row r="54" spans="2:12" ht="17" customHeight="1">
-      <c r="G54" s="127"/>
+      <c r="G54" s="129"/>
       <c r="H54" s="1" t="s">
         <v>7</v>
       </c>
@@ -3260,7 +3486,7 @@
       </c>
     </row>
     <row r="55" spans="2:12" ht="17" customHeight="1">
-      <c r="G55" s="127"/>
+      <c r="G55" s="129"/>
       <c r="H55" s="1" t="s">
         <v>6</v>
       </c>
@@ -3535,7 +3761,7 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AB73"/>
+  <dimension ref="B1:AB79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -3551,7 +3777,7 @@
     <row r="1" spans="2:8" ht="17" customHeight="1"/>
     <row r="2" spans="2:8" ht="17" customHeight="1">
       <c r="B2" s="38" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C2" s="24"/>
     </row>
@@ -3569,7 +3795,7 @@
     </row>
     <row r="5" spans="2:8" ht="17" customHeight="1">
       <c r="B5" s="110" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C5" s="24"/>
       <c r="F5" s="54"/>
@@ -3593,7 +3819,7 @@
     </row>
     <row r="8" spans="2:8" ht="17" customHeight="1">
       <c r="C8" s="20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D8" s="107">
         <v>17428496</v>
@@ -3673,13 +3899,13 @@
         <v>23</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H13" s="54"/>
     </row>
     <row r="14" spans="2:8" ht="17" customHeight="1">
       <c r="C14" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D14" s="80">
         <f>$L$52</f>
@@ -3690,13 +3916,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H14" s="54"/>
     </row>
     <row r="15" spans="2:8" ht="17" customHeight="1">
       <c r="C15" s="33" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D15" s="88">
         <f>D13*D14</f>
@@ -3737,13 +3963,13 @@
         <v>23</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="H18" s="54"/>
     </row>
     <row r="19" spans="3:8" ht="17" customHeight="1">
       <c r="C19" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D19" s="80">
         <f>$M$52</f>
@@ -3754,13 +3980,13 @@
         <v>0</v>
       </c>
       <c r="G19" s="106" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H19" s="54"/>
     </row>
     <row r="20" spans="3:8" ht="17" customHeight="1">
       <c r="C20" s="33" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D20" s="88">
         <f>D18*D19</f>
@@ -3801,7 +4027,7 @@
         <v>23</v>
       </c>
       <c r="G23" s="106" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="17" customHeight="1">
@@ -3835,7 +4061,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="53" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="17" customHeight="1" thickBot="1">
@@ -3875,22 +4101,22 @@
         <v>23</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="17" customHeight="1">
       <c r="C30" s="20" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D30" s="124">
         <f>$G$66</f>
-        <v>6.0833700516147024E-4</v>
+        <v>6.4101663635551668E-4</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="17" customHeight="1" thickBot="1">
@@ -3899,7 +4125,7 @@
       </c>
       <c r="D31" s="89">
         <f>D29*D30</f>
-        <v>6361.4394366651977</v>
+        <v>6703.1735295933458</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>24</v>
@@ -3923,28 +4149,28 @@
     </row>
     <row r="35" spans="2:28" ht="17" customHeight="1">
       <c r="B35" s="23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:28" ht="17" customHeight="1">
       <c r="B36" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G36" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" s="53" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" spans="2:28" ht="17" customHeight="1">
       <c r="B37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" s="53" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3952,10 +4178,10 @@
       <c r="B38" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G38" s="53" t="s">
+      <c r="E38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3978,7 +4204,7 @@
     </row>
     <row r="41" spans="2:28" ht="17" customHeight="1">
       <c r="B41" s="103" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H41"/>
       <c r="I41"/>
@@ -3995,37 +4221,37 @@
         <v>16</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E42" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="111" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F42" s="97" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="111" t="s">
-        <v>95</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="I42" s="24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J42" s="93" t="s">
         <v>85</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="N42" s="21"/>
       <c r="R42"/>
@@ -4050,6 +4276,7 @@
         <v>1776481</v>
       </c>
       <c r="G43" s="112">
+        <f>F43</f>
         <v>1776481</v>
       </c>
       <c r="H43" s="86">
@@ -4064,7 +4291,7 @@
         <f t="shared" ref="J43:J51" si="1">G43*C43*D43*E43</f>
         <v>7.4305833333333347</v>
       </c>
-      <c r="K43" s="100">
+      <c r="K43" s="127">
         <f>IF(G43&gt;0, H43/G43,"-")</f>
         <v>8.3655083655083673E-2</v>
       </c>
@@ -4073,7 +4300,7 @@
         <v>8.3655083655083658E-5</v>
       </c>
       <c r="M43" s="100">
-        <f t="shared" ref="M43:M51" si="3">IF(G43&gt;0, J43/G43,"-")</f>
+        <f t="shared" ref="M43:N51" si="3">IF(G43&gt;0, J43/G43,"-")</f>
         <v>4.1827541827541838E-6</v>
       </c>
       <c r="R43"/>
@@ -4097,10 +4324,11 @@
         <v>2001656</v>
       </c>
       <c r="G44" s="112">
+        <f t="shared" ref="G44:G47" si="4">F44</f>
         <v>2001656</v>
       </c>
       <c r="H44" s="86">
-        <f t="shared" ref="H44:H51" si="4">G44*C44</f>
+        <f t="shared" ref="H44:H51" si="5">G44*C44</f>
         <v>266629.85328185325</v>
       </c>
       <c r="I44" s="86">
@@ -4111,8 +4339,8 @@
         <f t="shared" si="1"/>
         <v>39.994477992277993</v>
       </c>
-      <c r="K44" s="100">
-        <f t="shared" ref="K44:K51" si="5">IF(G44&gt;0, H44/G44,"-")</f>
+      <c r="K44" s="127">
+        <f t="shared" ref="K44:K51" si="6">IF(G44&gt;0, H44/G44,"-")</f>
         <v>0.13320463320463319</v>
       </c>
       <c r="L44" s="101">
@@ -4144,10 +4372,11 @@
         <v>2244283</v>
       </c>
       <c r="G45" s="112">
+        <f t="shared" si="4"/>
         <v>2244283</v>
       </c>
       <c r="H45" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1171244.2168597167</v>
       </c>
       <c r="I45" s="86">
@@ -4158,8 +4387,8 @@
         <f t="shared" si="1"/>
         <v>702.74653011583007</v>
       </c>
-      <c r="K45" s="100">
-        <f t="shared" si="5"/>
+      <c r="K45" s="127">
+        <f t="shared" si="6"/>
         <v>0.5218790218790218</v>
       </c>
       <c r="L45" s="102">
@@ -4191,10 +4420,11 @@
         <v>2143651</v>
       </c>
       <c r="G46" s="112">
+        <f t="shared" si="4"/>
         <v>2143651</v>
       </c>
       <c r="H46" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1929837.6763191763</v>
       </c>
       <c r="I46" s="86">
@@ -4205,8 +4435,8 @@
         <f t="shared" si="1"/>
         <v>3087.7402821106825</v>
       </c>
-      <c r="K46" s="100">
-        <f t="shared" si="5"/>
+      <c r="K46" s="127">
+        <f t="shared" si="6"/>
         <v>0.90025740025740031</v>
       </c>
       <c r="L46" s="102">
@@ -4238,10 +4468,11 @@
         <v>2206346</v>
       </c>
       <c r="G47" s="112">
+        <f t="shared" si="4"/>
         <v>2206346</v>
       </c>
       <c r="H47" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1893993.2844272845</v>
       </c>
       <c r="I47" s="86">
@@ -4252,8 +4483,8 @@
         <f t="shared" si="1"/>
         <v>5846.7572690270281</v>
       </c>
-      <c r="K47" s="100">
-        <f t="shared" si="5"/>
+      <c r="K47" s="127">
+        <f t="shared" si="6"/>
         <v>0.85842985842985842</v>
       </c>
       <c r="L47" s="102">
@@ -4288,7 +4519,7 @@
         <v>84681</v>
       </c>
       <c r="H48" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84681</v>
       </c>
       <c r="I48" s="86">
@@ -4299,8 +4530,8 @@
         <f t="shared" si="1"/>
         <v>1053.770364</v>
       </c>
-      <c r="K48" s="100">
-        <f t="shared" si="5"/>
+      <c r="K48" s="127">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L48" s="102">
@@ -4335,7 +4566,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I49" s="86">
@@ -4346,8 +4577,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K49" s="100" t="str">
-        <f t="shared" si="5"/>
+      <c r="K49" s="127" t="str">
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="L49" s="102" t="str">
@@ -4382,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I50" s="86">
@@ -4393,8 +4624,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K50" s="100" t="str">
-        <f t="shared" si="5"/>
+      <c r="K50" s="127" t="str">
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="L50" s="102" t="str">
@@ -4430,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I51" s="86">
@@ -4441,8 +4672,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K51" s="100" t="str">
-        <f t="shared" si="5"/>
+      <c r="K51" s="127" t="str">
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="L51" s="102" t="str">
@@ -4459,7 +4690,7 @@
     </row>
     <row r="52" spans="2:28" ht="17" customHeight="1">
       <c r="B52" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="7"/>
@@ -4556,13 +4787,13 @@
         <v>16</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E56" s="111" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F56" s="111" t="s">
         <v>37</v>
@@ -4596,8 +4827,8 @@
       <c r="B57" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="79">
-        <v>2.0000000000000002E-5</v>
+      <c r="C57" s="130">
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="D57" s="98">
         <v>1776481</v>
@@ -4607,15 +4838,15 @@
         <v>1776481</v>
       </c>
       <c r="F57" s="117">
-        <f t="shared" ref="F57:F65" si="6">C57*E57</f>
-        <v>35.529620000000001</v>
-      </c>
-      <c r="G57" s="90">
-        <f t="shared" ref="G57:G65" si="7">IF(E57&gt;0, F57/E57,"-")</f>
-        <v>2.0000000000000002E-5</v>
+        <f t="shared" ref="F57:F65" si="7">C57*E57</f>
+        <v>28.423696</v>
+      </c>
+      <c r="G57" s="131">
+        <f t="shared" ref="G57:G65" si="8">IF(E57&gt;0, F57/E57,"-")</f>
+        <v>1.5999999999999999E-5</v>
       </c>
       <c r="H57" s="104" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I57"/>
       <c r="J57"/>
@@ -4643,25 +4874,25 @@
         <v>11</v>
       </c>
       <c r="C58" s="79">
-        <v>6.0000000000000002E-5</v>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="D58" s="98">
         <v>2001656</v>
       </c>
       <c r="E58" s="115">
-        <f t="shared" ref="E58:E65" si="8">G44</f>
+        <f t="shared" ref="E58:E65" si="9">G44</f>
         <v>2001656</v>
       </c>
       <c r="F58" s="117">
-        <f t="shared" si="6"/>
-        <v>120.09936</v>
+        <f t="shared" si="7"/>
+        <v>140.11591999999999</v>
       </c>
       <c r="G58" s="90">
-        <f t="shared" si="7"/>
-        <v>6.0000000000000002E-5</v>
+        <f t="shared" si="8"/>
+        <v>6.9999999999999994E-5</v>
       </c>
       <c r="H58" s="104" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I58"/>
       <c r="J58"/>
@@ -4689,22 +4920,22 @@
         <v>10</v>
       </c>
       <c r="C59" s="80">
-        <v>2.9999999999999997E-4</v>
+        <v>3.1E-4</v>
       </c>
       <c r="D59" s="98">
         <v>2244283</v>
       </c>
       <c r="E59" s="115">
+        <f t="shared" si="9"/>
+        <v>2244283</v>
+      </c>
+      <c r="F59" s="117">
+        <f t="shared" si="7"/>
+        <v>695.72772999999995</v>
+      </c>
+      <c r="G59" s="91">
         <f t="shared" si="8"/>
-        <v>2244283</v>
-      </c>
-      <c r="F59" s="117">
-        <f t="shared" si="6"/>
-        <v>673.28489999999999</v>
-      </c>
-      <c r="G59" s="91">
-        <f t="shared" si="7"/>
-        <v>2.9999999999999997E-4</v>
+        <v>3.1E-4</v>
       </c>
       <c r="H59" s="21"/>
       <c r="I59"/>
@@ -4733,22 +4964,22 @@
         <v>8</v>
       </c>
       <c r="C60" s="81">
-        <v>8.0000000000000004E-4</v>
+        <v>8.4000000000000003E-4</v>
       </c>
       <c r="D60" s="98">
         <v>2143651</v>
       </c>
       <c r="E60" s="115">
+        <f t="shared" si="9"/>
+        <v>2143651</v>
+      </c>
+      <c r="F60" s="117">
+        <f t="shared" si="7"/>
+        <v>1800.6668400000001</v>
+      </c>
+      <c r="G60" s="91">
         <f t="shared" si="8"/>
-        <v>2143651</v>
-      </c>
-      <c r="F60" s="117">
-        <f t="shared" si="6"/>
-        <v>1714.9208000000001</v>
-      </c>
-      <c r="G60" s="91">
-        <f t="shared" si="7"/>
-        <v>8.0000000000000004E-4</v>
+        <v>8.4000000000000003E-4</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
@@ -4777,22 +5008,22 @@
         <v>7</v>
       </c>
       <c r="C61" s="81">
-        <v>1.5E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D61" s="98">
         <v>2206346</v>
       </c>
       <c r="E61" s="115">
+        <f t="shared" si="9"/>
+        <v>2206346</v>
+      </c>
+      <c r="F61" s="117">
+        <f t="shared" si="7"/>
+        <v>3530.1536000000001</v>
+      </c>
+      <c r="G61" s="91">
         <f t="shared" si="8"/>
-        <v>2206346</v>
-      </c>
-      <c r="F61" s="117">
-        <f t="shared" si="6"/>
-        <v>3309.5190000000002</v>
-      </c>
-      <c r="G61" s="91">
-        <f t="shared" si="7"/>
-        <v>1.5E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
@@ -4827,15 +5058,15 @@
         <v>2531817</v>
       </c>
       <c r="E62" s="115">
+        <f t="shared" si="9"/>
+        <v>84681</v>
+      </c>
+      <c r="F62" s="117">
+        <f t="shared" si="7"/>
+        <v>508.08600000000001</v>
+      </c>
+      <c r="G62" s="91">
         <f t="shared" si="8"/>
-        <v>84681</v>
-      </c>
-      <c r="F62" s="117">
-        <f t="shared" si="6"/>
-        <v>508.08600000000001</v>
-      </c>
-      <c r="G62" s="91">
-        <f t="shared" si="7"/>
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="H62"/>
@@ -4871,15 +5102,15 @@
         <v>2114090</v>
       </c>
       <c r="E63" s="115">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="117">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G63" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F63" s="117">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="91" t="str">
-        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="H63"/>
@@ -4915,15 +5146,15 @@
         <v>1574580</v>
       </c>
       <c r="E64" s="115">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="117">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G64" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F64" s="117">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G64" s="91" t="str">
-        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="H64"/>
@@ -4960,15 +5191,15 @@
         <v>821695</v>
       </c>
       <c r="E65" s="115">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="117">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G65" s="91" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F65" s="117">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G65" s="91" t="str">
-        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="H65"/>
@@ -4995,7 +5226,7 @@
     </row>
     <row r="66" spans="2:28" ht="17" customHeight="1">
       <c r="B66" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C66" s="82"/>
       <c r="D66" s="99">
@@ -5008,11 +5239,11 @@
       </c>
       <c r="F66" s="114">
         <f>SUM(F57:F65)</f>
-        <v>6361.4396800000004</v>
+        <v>6703.1737860000003</v>
       </c>
       <c r="G66" s="116">
         <f>F66/E66</f>
-        <v>6.0833700516147024E-4</v>
+        <v>6.4101663635551668E-4</v>
       </c>
       <c r="H66"/>
       <c r="I66"/>
@@ -5068,27 +5299,47 @@
     <row r="68" spans="2:28" ht="17" customHeight="1"/>
     <row r="69" spans="2:28" ht="17" customHeight="1">
       <c r="B69" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="2:28">
       <c r="B70" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="2:28">
       <c r="B71" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="2:28">
       <c r="B72" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="2:28">
       <c r="B73" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="2:28" ht="16">
+      <c r="B76" s="103" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28">
+      <c r="B77" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28">
+      <c r="B78" s="126" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="2:28">
+      <c r="B79" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -5103,9 +5354,9 @@
     <hyperlink ref="G8" r:id="rId1"/>
     <hyperlink ref="G9" r:id="rId2"/>
     <hyperlink ref="G24" r:id="rId3"/>
-    <hyperlink ref="G38" r:id="rId4" location="/CBS/nl/dataset/84646NED/table?ts=1584394178496"/>
-    <hyperlink ref="G36" r:id="rId5"/>
-    <hyperlink ref="G37" r:id="rId6"/>
+    <hyperlink ref="H38" r:id="rId4" location="/CBS/nl/dataset/84646NED/table?ts=1584394178496"/>
+    <hyperlink ref="H36" r:id="rId5"/>
+    <hyperlink ref="H37" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39000000000000007" bottom="0.39000000000000007" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5321,7 +5572,7 @@
     </row>
     <row r="13" spans="2:14" ht="17" customHeight="1">
       <c r="C13" s="20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D13" s="35">
         <v>9.1999999999999998E-2</v>
@@ -5718,7 +5969,7 @@
         <f t="shared" si="1"/>
         <v>1.8E-3</v>
       </c>
-      <c r="G39" s="127" t="s">
+      <c r="G39" s="129" t="s">
         <v>9</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -5757,7 +6008,7 @@
         <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G40" s="127"/>
+      <c r="G40" s="129"/>
       <c r="H40" s="1" t="s">
         <v>7</v>
       </c>
@@ -5794,7 +6045,7 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G41" s="127"/>
+      <c r="G41" s="129"/>
       <c r="H41" s="1" t="s">
         <v>6</v>
       </c>
@@ -6041,7 +6292,7 @@
     <hyperlink ref="K13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -6113,11 +6364,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -6127,9 +6376,9 @@
     <col min="16" max="18" width="10.83203125" style="60"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="A1" s="77" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L1"/>
       <c r="M1"/>
@@ -6137,145 +6386,97 @@
       <c r="P1"/>
       <c r="Q1"/>
       <c r="R1"/>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="T1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="51" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="51"/>
       <c r="L2"/>
-      <c r="M2"/>
+      <c r="M2" s="51"/>
       <c r="O2"/>
       <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="51"/>
+      <c r="T2" s="53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="51" t="s">
+        <v>40</v>
+      </c>
       <c r="C3" s="51"/>
       <c r="L3"/>
-      <c r="M3"/>
+      <c r="M3" s="51"/>
       <c r="O3"/>
       <c r="P3"/>
       <c r="Q3"/>
       <c r="R3"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="78" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="58" t="s">
-        <v>92</v>
-      </c>
+      <c r="T3" s="53"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="L4"/>
-      <c r="M4"/>
+      <c r="M4" s="51"/>
       <c r="O4"/>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="R4"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="T4" s="53"/>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="78">
-        <f>B5+C5</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="58">
-        <f>B5/D5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="58">
-        <v>0</v>
-      </c>
-      <c r="G5" s="58">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="H5" s="58">
-        <f t="shared" ref="H5:H13" si="0">E5-F5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="58">
-        <f t="shared" ref="I5:I13" si="1">G5-E5</f>
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="J5" s="58">
-        <f t="shared" ref="J5:J13" si="2">AVERAGE(F5:G5)</f>
-        <v>0.48749999999999999</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C5" s="51"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
       <c r="R5"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="T5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U5" s="80">
+        <v>8.3655083655083659E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="78">
-        <f t="shared" ref="D6:D13" si="3">B6+C6</f>
-        <v>5</v>
-      </c>
-      <c r="E6" s="58">
-        <f t="shared" ref="E6:E13" si="4">B6/D6</f>
-        <v>0.4</v>
-      </c>
-      <c r="F6" s="58">
-        <v>5.2744949999999999E-2</v>
-      </c>
-      <c r="G6" s="58">
-        <v>0.85336719999999999</v>
-      </c>
-      <c r="H6" s="58">
-        <f t="shared" si="0"/>
-        <v>0.34725505000000001</v>
-      </c>
-      <c r="I6" s="58">
-        <f t="shared" si="1"/>
-        <v>0.45336719999999997</v>
-      </c>
-      <c r="J6" s="58">
-        <f t="shared" si="2"/>
-        <v>0.453056075</v>
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>90</v>
       </c>
       <c r="L6"/>
       <c r="M6"/>
@@ -6283,42 +6484,48 @@
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="T6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="U6" s="80">
+        <v>0.13320463320463319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" s="78">
-        <f t="shared" si="3"/>
-        <v>28</v>
+        <f>B7+C7</f>
+        <v>1</v>
       </c>
       <c r="E7" s="58">
-        <f t="shared" si="4"/>
-        <v>0.8928571428571429</v>
+        <f>B7/D7</f>
+        <v>0</v>
       </c>
       <c r="F7" s="58">
-        <v>0.71773560000000003</v>
+        <v>0</v>
       </c>
       <c r="G7" s="58">
-        <v>0.97733490000000001</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="H7" s="58">
-        <f t="shared" si="0"/>
-        <v>0.17512154285714288</v>
+        <f t="shared" ref="H7:H15" si="0">E7-F7</f>
+        <v>0</v>
       </c>
       <c r="I7" s="58">
-        <f t="shared" si="1"/>
-        <v>8.4477757142857102E-2</v>
+        <f t="shared" ref="I7:I15" si="1">G7-E7</f>
+        <v>0.97499999999999998</v>
       </c>
       <c r="J7" s="58">
-        <f t="shared" si="2"/>
-        <v>0.84753524999999996</v>
+        <f t="shared" ref="J7:J15" si="2">AVERAGE(F7:G7)</f>
+        <v>0.48749999999999999</v>
       </c>
       <c r="L7"/>
       <c r="M7"/>
@@ -6326,42 +6533,48 @@
       <c r="P7"/>
       <c r="Q7"/>
       <c r="R7"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="T7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="80">
+        <v>0.5218790218790218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="50" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="78">
-        <f t="shared" si="3"/>
-        <v>34</v>
+        <f t="shared" ref="D8:D15" si="3">B8+C8</f>
+        <v>5</v>
       </c>
       <c r="E8" s="58">
-        <f t="shared" si="4"/>
-        <v>0.79411764705882348</v>
+        <f t="shared" ref="E8:E15" si="4">B8/D8</f>
+        <v>0.4</v>
       </c>
       <c r="F8" s="58">
-        <v>0.62102230000000003</v>
+        <v>5.2744949999999999E-2</v>
       </c>
       <c r="G8" s="58">
-        <v>0.91297870000000003</v>
+        <v>0.85336719999999999</v>
       </c>
       <c r="H8" s="58">
         <f t="shared" si="0"/>
-        <v>0.17309534705882346</v>
+        <v>0.34725505000000001</v>
       </c>
       <c r="I8" s="58">
         <f t="shared" si="1"/>
-        <v>0.11886105294117655</v>
+        <v>0.45336719999999997</v>
       </c>
       <c r="J8" s="58">
         <f t="shared" si="2"/>
-        <v>0.76700049999999997</v>
+        <v>0.453056075</v>
       </c>
       <c r="L8"/>
       <c r="M8"/>
@@ -6369,42 +6582,48 @@
       <c r="P8"/>
       <c r="Q8"/>
       <c r="R8"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="T8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8" s="80">
+        <v>0.90025740025740031</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D9" s="78">
         <f t="shared" si="3"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="58">
         <f t="shared" si="4"/>
-        <v>0.70370370370370372</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="F9" s="58">
-        <v>0.49818630000000003</v>
+        <v>0.71773560000000003</v>
       </c>
       <c r="G9" s="58">
-        <v>0.86247339999999995</v>
+        <v>0.97733490000000001</v>
       </c>
       <c r="H9" s="58">
         <f t="shared" si="0"/>
-        <v>0.20551740370370369</v>
+        <v>0.17512154285714288</v>
       </c>
       <c r="I9" s="58">
         <f t="shared" si="1"/>
-        <v>0.15876969629629623</v>
+        <v>8.4477757142857102E-2</v>
       </c>
       <c r="J9" s="58">
         <f t="shared" si="2"/>
-        <v>0.68032985000000001</v>
+        <v>0.84753524999999996</v>
       </c>
       <c r="L9"/>
       <c r="M9"/>
@@ -6412,42 +6631,48 @@
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="T9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U9" s="80">
+        <v>0.85842985842985842</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D10" s="78">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E10" s="58">
         <f t="shared" si="4"/>
-        <v>0.47457627118644069</v>
+        <v>0.79411764705882348</v>
       </c>
       <c r="F10" s="58">
-        <v>0.3429836</v>
+        <v>0.62102230000000003</v>
       </c>
       <c r="G10" s="58">
-        <v>0.60880710000000005</v>
+        <v>0.91297870000000003</v>
       </c>
       <c r="H10" s="58">
         <f t="shared" si="0"/>
-        <v>0.13159267118644069</v>
+        <v>0.17309534705882346</v>
       </c>
       <c r="I10" s="58">
         <f t="shared" si="1"/>
-        <v>0.13423082881355936</v>
+        <v>0.11886105294117655</v>
       </c>
       <c r="J10" s="58">
         <f t="shared" si="2"/>
-        <v>0.47589535000000005</v>
+        <v>0.76700049999999997</v>
       </c>
       <c r="L10"/>
       <c r="M10"/>
@@ -6455,42 +6680,48 @@
       <c r="P10"/>
       <c r="Q10"/>
       <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="T10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="D11" s="78">
         <f t="shared" si="3"/>
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="E11" s="58">
         <f t="shared" si="4"/>
-        <v>0.42937853107344631</v>
+        <v>0.70370370370370372</v>
       </c>
       <c r="F11" s="58">
-        <v>0.35537190000000002</v>
+        <v>0.49818630000000003</v>
       </c>
       <c r="G11" s="58">
-        <v>0.50579090000000004</v>
+        <v>0.86247339999999995</v>
       </c>
       <c r="H11" s="58">
         <f t="shared" si="0"/>
-        <v>7.4006631073446294E-2</v>
+        <v>0.20551740370370369</v>
       </c>
       <c r="I11" s="58">
         <f t="shared" si="1"/>
-        <v>7.6412368926553731E-2</v>
+        <v>0.15876969629629623</v>
       </c>
       <c r="J11" s="58">
         <f t="shared" si="2"/>
-        <v>0.4305814</v>
+        <v>0.68032985000000001</v>
       </c>
       <c r="L11"/>
       <c r="M11"/>
@@ -6498,42 +6729,48 @@
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="T11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U11" s="80">
+        <v>0.48970398970398971</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="C12">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="D12" s="78">
         <f t="shared" si="3"/>
-        <v>234</v>
+        <v>59</v>
       </c>
       <c r="E12" s="58">
         <f t="shared" si="4"/>
-        <v>0.40598290598290598</v>
+        <v>0.47457627118644069</v>
       </c>
       <c r="F12" s="58">
-        <v>0.34247650000000002</v>
+        <v>0.3429836</v>
       </c>
       <c r="G12" s="58">
-        <v>0.47190280000000001</v>
+        <v>0.60880710000000005</v>
       </c>
       <c r="H12" s="58">
         <f t="shared" si="0"/>
-        <v>6.3506405982905967E-2</v>
+        <v>0.13159267118644069</v>
       </c>
       <c r="I12" s="58">
         <f t="shared" si="1"/>
-        <v>6.5919894017094027E-2</v>
+        <v>0.13423082881355936</v>
       </c>
       <c r="J12" s="58">
         <f t="shared" si="2"/>
-        <v>0.40718965000000001</v>
+        <v>0.47589535000000005</v>
       </c>
       <c r="L12"/>
       <c r="M12"/>
@@ -6541,42 +6778,48 @@
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="T12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="80">
+        <v>0.40604890604890603</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C13">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="D13" s="78">
         <f t="shared" si="3"/>
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="E13" s="58">
         <f t="shared" si="4"/>
-        <v>0.53703703703703709</v>
+        <v>0.42937853107344631</v>
       </c>
       <c r="F13" s="58">
-        <v>0.39609499999999997</v>
+        <v>0.35537190000000002</v>
       </c>
       <c r="G13" s="58">
-        <v>0.67377540000000002</v>
+        <v>0.50579090000000004</v>
       </c>
       <c r="H13" s="58">
         <f t="shared" si="0"/>
-        <v>0.14094203703703712</v>
+        <v>7.4006631073446294E-2</v>
       </c>
       <c r="I13" s="58">
         <f t="shared" si="1"/>
-        <v>0.13673836296296293</v>
+        <v>7.6412368926553731E-2</v>
       </c>
       <c r="J13" s="58">
         <f t="shared" si="2"/>
-        <v>0.53493520000000006</v>
+        <v>0.4305814</v>
       </c>
       <c r="L13"/>
       <c r="M13"/>
@@ -6584,9 +6827,49 @@
       <c r="P13"/>
       <c r="Q13"/>
       <c r="R13"/>
-    </row>
-    <row r="14" spans="1:18">
-      <c r="A14" s="50"/>
+      <c r="T13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U13" s="96">
+        <v>0.16795366795366795</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>139</v>
+      </c>
+      <c r="D14" s="78">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+      <c r="E14" s="58">
+        <f t="shared" si="4"/>
+        <v>0.40598290598290598</v>
+      </c>
+      <c r="F14" s="58">
+        <v>0.34247650000000002</v>
+      </c>
+      <c r="G14" s="58">
+        <v>0.47190280000000001</v>
+      </c>
+      <c r="H14" s="58">
+        <f t="shared" si="0"/>
+        <v>6.3506405982905967E-2</v>
+      </c>
+      <c r="I14" s="58">
+        <f t="shared" si="1"/>
+        <v>6.5919894017094027E-2</v>
+      </c>
+      <c r="J14" s="58">
+        <f t="shared" si="2"/>
+        <v>0.40718965000000001</v>
+      </c>
       <c r="L14"/>
       <c r="M14"/>
       <c r="O14"/>
@@ -6594,7 +6877,42 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:21">
+      <c r="A15" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15" s="78">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="E15" s="58">
+        <f t="shared" si="4"/>
+        <v>0.53703703703703709</v>
+      </c>
+      <c r="F15" s="58">
+        <v>0.39609499999999997</v>
+      </c>
+      <c r="G15" s="58">
+        <v>0.67377540000000002</v>
+      </c>
+      <c r="H15" s="58">
+        <f t="shared" si="0"/>
+        <v>0.14094203703703712</v>
+      </c>
+      <c r="I15" s="58">
+        <f t="shared" si="1"/>
+        <v>0.13673836296296293</v>
+      </c>
+      <c r="J15" s="58">
+        <f t="shared" si="2"/>
+        <v>0.53493520000000006</v>
+      </c>
       <c r="L15"/>
       <c r="M15"/>
       <c r="O15"/>
@@ -6602,7 +6920,8 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:21">
+      <c r="A16" s="50"/>
       <c r="L16"/>
       <c r="M16"/>
       <c r="O16"/>
@@ -6618,12 +6937,31 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
+    <row r="18" spans="12:18">
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+    </row>
+    <row r="19" spans="12:18">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
op korte termijn meer bedden beschikbaar
</commit_message>
<xml_diff>
--- a/IC-capaciteit.xlsx
+++ b/IC-capaciteit.xlsx
@@ -1142,15 +1142,15 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="166">
@@ -1788,11 +1788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2117780200"/>
-        <c:axId val="2117783400"/>
+        <c:axId val="-2139980856"/>
+        <c:axId val="-2145702808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2117780200"/>
+        <c:axId val="-2139980856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,7 +1801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117783400"/>
+        <c:crossAx val="-2145702808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1809,7 +1809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117783400"/>
+        <c:axId val="-2145702808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1832,21 +1832,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117780200"/>
+        <c:crossAx val="-2139980856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2861,7 +2859,7 @@
         <f t="shared" si="1"/>
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="G39" s="128" t="s">
+      <c r="G39" s="130" t="s">
         <v>73</v>
       </c>
       <c r="H39" s="14" t="s">
@@ -2938,7 +2936,7 @@
         <f t="shared" si="1"/>
         <v>1.5E-3</v>
       </c>
-      <c r="G40" s="128"/>
+      <c r="G40" s="130"/>
       <c r="H40" s="14" t="s">
         <v>7</v>
       </c>
@@ -3013,7 +3011,7 @@
         <f t="shared" si="1"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G41" s="128"/>
+      <c r="G41" s="130"/>
       <c r="H41" s="14" t="s">
         <v>6</v>
       </c>
@@ -3456,7 +3454,7 @@
       </c>
     </row>
     <row r="53" spans="2:12" ht="17" customHeight="1">
-      <c r="G53" s="129" t="s">
+      <c r="G53" s="131" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="1" t="s">
@@ -3478,7 +3476,7 @@
       </c>
     </row>
     <row r="54" spans="2:12" ht="17" customHeight="1">
-      <c r="G54" s="129"/>
+      <c r="G54" s="131"/>
       <c r="H54" s="1" t="s">
         <v>7</v>
       </c>
@@ -3498,7 +3496,7 @@
       </c>
     </row>
     <row r="55" spans="2:12" ht="17" customHeight="1">
-      <c r="G55" s="129"/>
+      <c r="G55" s="131"/>
       <c r="H55" s="1" t="s">
         <v>6</v>
       </c>
@@ -3776,7 +3774,7 @@
   <dimension ref="B1:AB79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4066,8 +4064,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="28">
-        <f>1150-575</f>
-        <v>575</v>
+        <v>925</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>20</v>
@@ -4085,7 +4082,7 @@
       </c>
       <c r="D26" s="89">
         <f>D23*D24/D25</f>
-        <v>280.13320451945611</v>
+        <v>174.1368568634457</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>17</v>
@@ -4315,7 +4312,7 @@
         <v>8.3655083655083658E-5</v>
       </c>
       <c r="M43" s="100">
-        <f t="shared" ref="M43:N51" si="3">IF(G43&gt;0, J43/G43,"-")</f>
+        <f t="shared" ref="M43:M51" si="3">IF(G43&gt;0, J43/G43,"-")</f>
         <v>4.1827541827541838E-6</v>
       </c>
       <c r="R43"/>
@@ -4842,7 +4839,7 @@
       <c r="B57" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="130">
+      <c r="C57" s="128">
         <v>1.5999999999999999E-5</v>
       </c>
       <c r="D57" s="98">
@@ -4856,7 +4853,7 @@
         <f t="shared" ref="F57:F65" si="7">C57*E57</f>
         <v>28.423696</v>
       </c>
-      <c r="G57" s="131">
+      <c r="G57" s="129">
         <f t="shared" ref="G57:G65" si="8">IF(E57&gt;0, F57/E57,"-")</f>
         <v>1.5999999999999999E-5</v>
       </c>
@@ -5373,7 +5370,6 @@
     <hyperlink ref="H37" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39000000000000007" bottom="0.39000000000000007" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -5985,7 +5981,7 @@
         <f t="shared" si="1"/>
         <v>1.8E-3</v>
       </c>
-      <c r="G39" s="129" t="s">
+      <c r="G39" s="131" t="s">
         <v>9</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -6024,7 +6020,7 @@
         <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G40" s="129"/>
+      <c r="G40" s="131"/>
       <c r="H40" s="1" t="s">
         <v>7</v>
       </c>
@@ -6061,7 +6057,7 @@
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G41" s="129"/>
+      <c r="G41" s="131"/>
       <c r="H41" s="1" t="s">
         <v>6</v>
       </c>
@@ -6308,7 +6304,6 @@
     <hyperlink ref="K13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -6957,7 +6952,6 @@
     <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
automatic selection of youngest population
</commit_message>
<xml_diff>
--- a/IC-capaciteit.xlsx
+++ b/IC-capaciteit.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COVID.calc.groepsimmuniteit (3)" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="151">
   <si>
     <t>=</t>
   </si>
@@ -444,9 +444,6 @@
     <t>IFR gekozen populatie</t>
   </si>
   <si>
-    <t>Kies de besmette populatie in cel G43:G51</t>
-  </si>
-  <si>
     <t>ascertainment rate in studie IC load</t>
   </si>
   <si>
@@ -490,6 +487,36 @@
   </si>
   <si>
     <t>https://www.rijksoverheid.nl/binaries/rijksoverheid/documenten/kamerstukken/2020/03/20/kamerbrief-covid-19-update-stand-van-zaken/COVID-19+-+Update+stand+van+zaken.pdf</t>
+  </si>
+  <si>
+    <t>China, jan 29 = bovengrens 95%CI bij 55 IC-patiënten uit 1099 cases:</t>
+  </si>
+  <si>
+    <t>Wuhan tot jan 29-31 = 9,2% (95%CI: 5,0-20,0), alternatief: Wuhan jan 1-22 = 5.0% (3,6–7,4)</t>
+  </si>
+  <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>totaal</t>
+  </si>
+  <si>
+    <t>80-89</t>
+  </si>
+  <si>
+    <t>Iceland 29 March</t>
+  </si>
+  <si>
+    <t>90+</t>
+  </si>
+  <si>
+    <t>infected</t>
+  </si>
+  <si>
+    <t>Deze rekenmethode neemt aan dat IC-belasting per leeftijd vergelijkbaar is met sterftekans per leeftijd. Dat is niet realistisch gebleken: hoogste leeftijdsgroepen belanden minder op IC. Daarom wordt in de tweede methode de IC-kans apart onderzocht.</t>
+  </si>
+  <si>
+    <t>Automatisch wordt een zo jong mogelijke besmette populatie gekozen in cel G43:G51. Deze cellen zijn ook handmatig aan te passen.</t>
   </si>
 </sst>
 </file>
@@ -502,7 +529,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -611,6 +638,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue Light"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue Light"/>
     </font>
   </fonts>
@@ -769,7 +802,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="166">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -936,8 +969,31 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1152,8 +1208,9 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="166">
+  <cellStyles count="189">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1318,6 +1375,29 @@
     <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1437,7 +1517,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
+              <c:f>'Diamond Princess'!$A$7:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1610,7 +1690,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
+              <c:f>'Diamond Princess'!$A$7:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1707,7 +1787,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Diamond Princess'!$T$5:$T$13</c:f>
+              <c:f>'Diamond Princess'!$A$7:$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1742,10 +1822,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Diamond Princess'!$J$7:$J$15</c:f>
+              <c:f>'Diamond Princess'!$J$7:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.4875</c:v>
                 </c:pt>
@@ -1788,11 +1868,123 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2139980856"/>
-        <c:axId val="-2145702808"/>
+        <c:axId val="2089923304"/>
+        <c:axId val="2089920344"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iceland 29 March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Diamond Princess'!$L$7:$L$16</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30-39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40-49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50-59</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60-69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70-79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80-89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90+</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Diamond Princess'!$O$7:$O$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.00048090134652377</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00171677697711717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00327542601268709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00368026859504132</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00530242597719487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00449427571198789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00357581547700286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00166494172703955</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.000389939559368298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00251677852348993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2131717608"/>
+        <c:axId val="2120912424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2139980856"/>
+        <c:axId val="2089923304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1801,7 +1993,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145702808"/>
+        <c:crossAx val="2089920344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1809,7 +2001,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145702808"/>
+        <c:axId val="2089920344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1832,19 +2024,53 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2139980856"/>
+        <c:crossAx val="2089923304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="2120912424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131717608"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2131717608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2120912424"/>
+        <c:crosses val="max"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3773,9 +3999,7 @@
   </sheetPr>
   <dimension ref="B1:AB79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -3807,7 +4031,7 @@
     </row>
     <row r="5" spans="2:8" ht="17" customHeight="1">
       <c r="B5" s="110" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="C5" s="24"/>
       <c r="F5" s="54"/>
@@ -3834,7 +4058,7 @@
         <v>119</v>
       </c>
       <c r="D8" s="107">
-        <v>17428496</v>
+        <v>90000000</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -3868,7 +4092,7 @@
       </c>
       <c r="D10" s="108">
         <f>D8*D9</f>
-        <v>10457097.6</v>
+        <v>54000000</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>24</v>
@@ -3876,7 +4100,7 @@
       <c r="F10" s="57"/>
       <c r="G10" s="109" t="str">
         <f>IF(ABS(D10-G52)&lt;1,"✅ de gekozen populatie in cel G52 is gelijk aan dit aantal personen",IF(D10&lt;G52,"✅ de gekozen populatie in cel G52 is groter dan dit aantal personen","❗ de gekozen populatie in cel G52 is kleiner dan dit aantal personen!"))</f>
-        <v>✅ de gekozen populatie in cel G52 is gelijk aan dit aantal personen</v>
+        <v>❗ de gekozen populatie in cel G52 is kleiner dan dit aantal personen!</v>
       </c>
       <c r="H10" s="54"/>
     </row>
@@ -3902,7 +4126,7 @@
       </c>
       <c r="D13" s="87">
         <f>$D$10</f>
-        <v>10457097.6</v>
+        <v>54000000</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>24</v>
@@ -3921,7 +4145,7 @@
       </c>
       <c r="D14" s="80">
         <f>$L$52</f>
-        <v>1.7041187756677751E-2</v>
+        <v>3.3152625906193223E-2</v>
       </c>
       <c r="E14" s="21"/>
       <c r="F14" s="19" t="s">
@@ -3938,7 +4162,7 @@
       </c>
       <c r="D15" s="88">
         <f>D13*D14</f>
-        <v>178201.36359150428</v>
+        <v>1790241.7989344341</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>24</v>
@@ -3966,7 +4190,7 @@
       </c>
       <c r="D18" s="87">
         <f>$D$10</f>
-        <v>10457097.6</v>
+        <v>54000000</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>24</v>
@@ -3985,7 +4209,7 @@
       </c>
       <c r="D19" s="80">
         <f>$M$52</f>
-        <v>1.0269043578418364E-3</v>
+        <v>3.1920220828744387E-3</v>
       </c>
       <c r="E19" s="43"/>
       <c r="F19" s="19" t="s">
@@ -4002,7 +4226,7 @@
       </c>
       <c r="D20" s="88">
         <f>D18*D19</f>
-        <v>10738.439095817408</v>
+        <v>172369.19247521969</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>24</v>
@@ -4030,7 +4254,7 @@
       </c>
       <c r="D23" s="86">
         <f>$J$52</f>
-        <v>10738.439506579152</v>
+        <v>41190.599890579149</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>24</v>
@@ -4073,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="17" customHeight="1" thickBot="1">
@@ -4082,7 +4306,7 @@
       </c>
       <c r="D26" s="89">
         <f>D23*D24/D25</f>
-        <v>174.1368568634457</v>
+        <v>667.95567390128349</v>
       </c>
       <c r="E26" s="25" t="s">
         <v>17</v>
@@ -4104,7 +4328,7 @@
       </c>
       <c r="D29" s="87">
         <f>$D$10</f>
-        <v>10457097.6</v>
+        <v>54000000</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>24</v>
@@ -4122,7 +4346,7 @@
       </c>
       <c r="D30" s="124">
         <f>$G$66</f>
-        <v>6.4101663635551668E-4</v>
+        <v>1.289821171225361E-2</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>0</v>
@@ -4137,7 +4361,7 @@
       </c>
       <c r="D31" s="89">
         <f>D29*D30</f>
-        <v>6703.1735295933458</v>
+        <v>696503.43246169493</v>
       </c>
       <c r="E31" s="46" t="s">
         <v>24</v>
@@ -4166,10 +4390,10 @@
     </row>
     <row r="36" spans="2:28" ht="17" customHeight="1">
       <c r="B36" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H36" s="53" t="s">
         <v>74</v>
@@ -4177,10 +4401,10 @@
     </row>
     <row r="37" spans="2:28" ht="17" customHeight="1">
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H37" s="53" t="s">
         <v>75</v>
@@ -4336,7 +4560,7 @@
         <v>2001656</v>
       </c>
       <c r="G44" s="112">
-        <f t="shared" ref="G44:G47" si="4">F44</f>
+        <f t="shared" ref="G44:G51" si="4">F44</f>
         <v>2001656</v>
       </c>
       <c r="H44" s="86">
@@ -4528,19 +4752,20 @@
         <v>2531817</v>
       </c>
       <c r="G48" s="112">
-        <v>84681</v>
+        <f t="shared" si="4"/>
+        <v>2531817</v>
       </c>
       <c r="H48" s="86">
         <f t="shared" si="5"/>
-        <v>84681</v>
+        <v>2531817</v>
       </c>
       <c r="I48" s="86">
         <f t="shared" si="0"/>
-        <v>8637.4619999999995</v>
+        <v>258245.33399999997</v>
       </c>
       <c r="J48" s="85">
         <f t="shared" si="1"/>
-        <v>1053.770364</v>
+        <v>31505.930747999995</v>
       </c>
       <c r="K48" s="127">
         <f t="shared" si="6"/>
@@ -4552,7 +4777,7 @@
       </c>
       <c r="M48" s="102">
         <f t="shared" si="3"/>
-        <v>1.2444E-2</v>
+        <v>1.2443999999999998E-2</v>
       </c>
       <c r="R48"/>
       <c r="S48"/>
@@ -4713,31 +4938,31 @@
       </c>
       <c r="G52" s="113">
         <f>SUM(G43:G51)</f>
-        <v>10457098</v>
+        <v>12904234</v>
       </c>
       <c r="H52" s="118">
         <f>SUM(H43:H51)</f>
-        <v>5494997.6975546973</v>
+        <v>7942133.6975546973</v>
       </c>
       <c r="I52" s="118">
         <f>SUM(I43:I51)</f>
-        <v>178201.37040797941</v>
+        <v>427809.24240797939</v>
       </c>
       <c r="J52" s="119">
         <f>SUM(J43:J51)</f>
-        <v>10738.439506579152</v>
+        <v>41190.599890579149</v>
       </c>
       <c r="K52" s="120">
         <f>H52/G52</f>
-        <v>0.52548017600625885</v>
+        <v>0.61546727202518936</v>
       </c>
       <c r="L52" s="120">
         <f>I52/G52</f>
-        <v>1.7041187756677751E-2</v>
+        <v>3.3152625906193223E-2</v>
       </c>
       <c r="M52" s="120">
         <f>J52/G52</f>
-        <v>1.0269043578418364E-3</v>
+        <v>3.1920220828744387E-3</v>
       </c>
       <c r="R52"/>
       <c r="S52"/>
@@ -4892,7 +5117,7 @@
         <v>2001656</v>
       </c>
       <c r="E58" s="115">
-        <f t="shared" ref="E58:E65" si="9">G44</f>
+        <f t="shared" ref="E58:E61" si="9">G44</f>
         <v>2001656</v>
       </c>
       <c r="F58" s="117">
@@ -5069,13 +5294,12 @@
       <c r="D62" s="98">
         <v>2531817</v>
       </c>
-      <c r="E62" s="115">
-        <f t="shared" si="9"/>
-        <v>84681</v>
+      <c r="E62" s="98">
+        <v>2531817</v>
       </c>
       <c r="F62" s="117">
         <f t="shared" si="7"/>
-        <v>508.08600000000001</v>
+        <v>15190.902</v>
       </c>
       <c r="G62" s="91">
         <f t="shared" si="8"/>
@@ -5113,17 +5337,16 @@
       <c r="D63" s="98">
         <v>2114090</v>
       </c>
-      <c r="E63" s="115">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="E63" s="98">
+        <v>2114090</v>
       </c>
       <c r="F63" s="117">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G63" s="91" t="str">
+        <v>46509.979999999996</v>
+      </c>
+      <c r="G63" s="91">
         <f t="shared" si="8"/>
-        <v>-</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H63"/>
       <c r="I63"/>
@@ -5157,17 +5380,16 @@
       <c r="D64" s="98">
         <v>1574580</v>
       </c>
-      <c r="E64" s="115">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="E64" s="98">
+        <v>1574580</v>
       </c>
       <c r="F64" s="117">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G64" s="91" t="str">
+        <v>80303.58</v>
+      </c>
+      <c r="G64" s="91">
         <f t="shared" si="8"/>
-        <v>-</v>
+        <v>5.1000000000000004E-2</v>
       </c>
       <c r="H64"/>
       <c r="I64"/>
@@ -5202,17 +5424,17 @@
         <f>691995+129700</f>
         <v>821695</v>
       </c>
-      <c r="E65" s="115">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="E65" s="98">
+        <f>691995+129700</f>
+        <v>821695</v>
       </c>
       <c r="F65" s="117">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="G65" s="91" t="str">
+        <v>76417.634999999995</v>
+      </c>
+      <c r="G65" s="91">
         <f t="shared" si="8"/>
-        <v>-</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="H65"/>
       <c r="I65"/>
@@ -5247,15 +5469,15 @@
       </c>
       <c r="E66" s="92">
         <f>SUM(E57:E65)</f>
-        <v>10457098</v>
+        <v>17414599</v>
       </c>
       <c r="F66" s="114">
         <f>SUM(F57:F65)</f>
-        <v>6703.1737860000003</v>
+        <v>224617.184786</v>
       </c>
       <c r="G66" s="116">
         <f>F66/E66</f>
-        <v>6.4101663635551668E-4</v>
+        <v>1.289821171225361E-2</v>
       </c>
       <c r="H66"/>
       <c r="I66"/>
@@ -5336,25 +5558,26 @@
     </row>
     <row r="76" spans="2:28" ht="16">
       <c r="B76" s="103" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="2:28">
       <c r="B77" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="2:28">
       <c r="B78" s="126" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="2:28">
       <c r="B79" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="G10:K10">
     <cfRule type="expression" dxfId="3" priority="1">
@@ -5370,6 +5593,7 @@
     <hyperlink ref="H37" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39000000000000007" bottom="0.39000000000000007" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -5409,7 +5633,7 @@
               <x14:cfIcon iconSet="3Stars" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E57:E65</xm:sqref>
+          <xm:sqref>E57:E61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{28BE3ED3-F3A6-2345-A516-A200396592F2}">
@@ -5444,11 +5668,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N56"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -5456,725 +5678,658 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="17" customHeight="1"/>
-    <row r="2" spans="2:14" ht="17" customHeight="1">
-      <c r="B2" s="38" t="s">
+    <row r="1" spans="1:16" ht="17" customHeight="1"/>
+    <row r="2" spans="1:16" ht="17" customHeight="1">
+      <c r="A2" s="132" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" customHeight="1">
+      <c r="A3" s="132"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" customHeight="1">
+      <c r="B4" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3" spans="2:14" ht="17" customHeight="1">
-      <c r="B3" s="37" t="s">
+      <c r="C4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" ht="17" customHeight="1">
+      <c r="B5" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="24"/>
-    </row>
-    <row r="4" spans="2:14" ht="17" customHeight="1">
-      <c r="B4" s="37" t="s">
+      <c r="C5" s="24"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" customHeight="1">
+      <c r="B6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="24"/>
-    </row>
-    <row r="5" spans="2:14" ht="17" customHeight="1">
-      <c r="B5" s="37"/>
-      <c r="C5" s="24"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-    </row>
-    <row r="6" spans="2:14" ht="17" customHeight="1">
       <c r="C6" s="24"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55" t="s">
+    </row>
+    <row r="7" spans="1:16" ht="17" customHeight="1">
+      <c r="B7" s="37"/>
+      <c r="C7" s="24"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+    </row>
+    <row r="8" spans="1:16" ht="17" customHeight="1">
+      <c r="C8" s="24"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="54"/>
-    </row>
-    <row r="7" spans="2:14" ht="17" customHeight="1">
-      <c r="C7" s="20" t="s">
+      <c r="H8" s="54"/>
+    </row>
+    <row r="9" spans="1:16" ht="17" customHeight="1">
+      <c r="C9" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D9" s="1">
         <v>17428496</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F9" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="56" t="s">
+      <c r="G9" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="54"/>
-    </row>
-    <row r="8" spans="2:14" ht="17" customHeight="1">
-      <c r="C8" s="20" t="s">
+      <c r="H9" s="54"/>
+    </row>
+    <row r="10" spans="1:16" ht="17" customHeight="1">
+      <c r="C10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D10" s="36">
         <v>0.6</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F10" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G10" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="54"/>
-    </row>
-    <row r="9" spans="2:14" ht="17" customHeight="1">
-      <c r="C9" s="33" t="s">
+      <c r="H10" s="54"/>
+    </row>
+    <row r="11" spans="1:16" ht="17" customHeight="1">
+      <c r="C11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="47">
-        <f>D7*D8</f>
+      <c r="D11" s="47">
+        <f>D9*D10</f>
         <v>10457097.6</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E11" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-    </row>
-    <row r="10" spans="2:14" ht="17" customHeight="1">
-      <c r="C10" s="20"/>
-      <c r="D10" s="32"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-    </row>
-    <row r="11" spans="2:14" ht="17" customHeight="1">
-      <c r="C11" s="20" t="s">
+      <c r="F11" s="57"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+    </row>
+    <row r="12" spans="1:16" ht="17" customHeight="1">
+      <c r="C12" s="20"/>
+      <c r="D12" s="32"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+    </row>
+    <row r="13" spans="1:16" ht="17" customHeight="1">
+      <c r="C13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="29">
-        <f>D9</f>
+      <c r="D13" s="29">
+        <f>D11</f>
         <v>10457097.6</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F13" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="54" t="s">
+      <c r="G13" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="54"/>
-    </row>
-    <row r="12" spans="2:14" ht="17" customHeight="1">
-      <c r="C12" s="20" t="s">
+      <c r="H13" s="54"/>
+    </row>
+    <row r="14" spans="1:16" ht="17" customHeight="1">
+      <c r="C14" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D14" s="35">
         <v>6.4645889999999998E-2</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F14" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="54"/>
-      <c r="K12" s="53" t="s">
+      <c r="G14" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14" s="54"/>
+      <c r="L14" s="53" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="17" customHeight="1">
-      <c r="C13" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D13" s="35">
+    <row r="15" spans="1:16" ht="17" customHeight="1">
+      <c r="C15" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="35">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F15" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="54" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="54"/>
-      <c r="K13" s="53" t="s">
+      <c r="G15" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="M15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="N13" s="53" t="s">
+      <c r="P15" s="53" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="17" customHeight="1">
-      <c r="C14" s="20" t="s">
+    <row r="16" spans="1:16" ht="17" customHeight="1">
+      <c r="C16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="34">
-        <f>B53</f>
+      <c r="D16" s="34">
+        <f>B55</f>
         <v>6.0945326299056038E-2</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F16" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G14" s="54" t="s">
+      <c r="G16" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="54"/>
-    </row>
-    <row r="15" spans="2:14" ht="17" customHeight="1">
-      <c r="C15" s="33" t="s">
+      <c r="H16" s="54"/>
+    </row>
+    <row r="17" spans="2:8" ht="17" customHeight="1">
+      <c r="C17" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="31">
-        <f>D11*D13*D12*D14</f>
+      <c r="D17" s="31">
+        <f>D13*D15*D14*D16</f>
         <v>3790.3587261534417</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-    </row>
-    <row r="16" spans="2:14" ht="17" customHeight="1">
-      <c r="C16" s="24"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-    </row>
-    <row r="17" spans="2:7" ht="17" customHeight="1">
-      <c r="C17" s="24" t="s">
+      <c r="F17" s="57"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+    </row>
+    <row r="18" spans="2:8" ht="17" customHeight="1">
+      <c r="C18" s="24"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+    </row>
+    <row r="19" spans="2:8" ht="17" customHeight="1">
+      <c r="C19" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D19" s="32">
+        <f>D17</f>
+        <v>3790.3587261534417</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="17" customHeight="1">
+      <c r="C20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="28">
+        <v>15</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="17" customHeight="1">
+      <c r="C21" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="28">
+        <v>850</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="17" customHeight="1" thickBot="1">
+      <c r="C22" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="26">
+        <f>D19*D20/D21</f>
+        <v>66.888683402707798</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="17" customHeight="1" thickTop="1">
+      <c r="C23" s="27"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
+    </row>
+    <row r="24" spans="2:8" ht="17" customHeight="1">
+      <c r="C24" s="27"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42"/>
+    </row>
+    <row r="25" spans="2:8" ht="17" customHeight="1">
+      <c r="C25" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="29">
+        <f>D11</f>
+        <v>10457097.6</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="17" customHeight="1">
+      <c r="C26" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="44">
         <f>D15</f>
-        <v>3790.3587261534417</v>
-      </c>
-      <c r="E17" s="1" t="s">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="17" customHeight="1">
+      <c r="C27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="35">
+        <f>L47</f>
+        <v>1.5666528897405377E-3</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="17" customHeight="1" thickBot="1">
+      <c r="C28" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="26">
+        <f>D25*D26*D27</f>
+        <v>1507.2030799471734</v>
+      </c>
+      <c r="E28" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="17" customHeight="1">
-      <c r="C18" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="28">
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="2:8" ht="17" customHeight="1" thickTop="1">
+      <c r="C29" s="33"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="2:8" ht="17" customHeight="1">
+      <c r="C30" s="33"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="2:8" ht="17" customHeight="1">
+      <c r="C31" s="24"/>
+    </row>
+    <row r="32" spans="2:8" ht="17" customHeight="1">
+      <c r="B32" s="23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="17" customHeight="1">
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="17" customHeight="1">
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="17" customHeight="1"/>
+    <row r="36" spans="2:12" ht="17" customHeight="1">
+      <c r="B36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="17" customHeight="1">
+      <c r="B37" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="53" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="17" customHeight="1">
-      <c r="C19" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="28">
-        <v>850</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="53" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="17" customHeight="1" thickBot="1">
-      <c r="C20" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="26">
-        <f>D17*D18/D19</f>
-        <v>66.888683402707798</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="17" customHeight="1" thickTop="1">
-      <c r="C21" s="27"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
-    </row>
-    <row r="22" spans="2:7" ht="17" customHeight="1">
-      <c r="C22" s="27"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-    </row>
-    <row r="23" spans="2:7" ht="17" customHeight="1">
-      <c r="C23" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="29">
-        <f>D9</f>
-        <v>10457097.6</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="17" customHeight="1">
-      <c r="C24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="44">
-        <f>D13</f>
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="17" customHeight="1">
-      <c r="C25" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="35">
-        <f>L45</f>
-        <v>1.5666528897405377E-3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G25" s="52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="17" customHeight="1" thickBot="1">
-      <c r="C26" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="26">
-        <f>D23*D24*D25</f>
-        <v>1507.2030799471734</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="19"/>
-    </row>
-    <row r="27" spans="2:7" ht="17" customHeight="1" thickTop="1">
-      <c r="C27" s="33"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" spans="2:7" ht="17" customHeight="1">
-      <c r="C28" s="33"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" spans="2:7" ht="17" customHeight="1">
-      <c r="C29" s="24"/>
-    </row>
-    <row r="30" spans="2:7" ht="17" customHeight="1">
-      <c r="B30" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="17" customHeight="1">
-      <c r="B31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="53" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="17" customHeight="1">
-      <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="53" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" ht="17" customHeight="1"/>
-    <row r="34" spans="2:12" ht="17" customHeight="1">
-      <c r="B34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" ht="17" customHeight="1">
-      <c r="B35" s="21" t="s">
+      <c r="D37" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="I37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="J37" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="K37" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="L37" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="L35" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="17" customHeight="1">
-      <c r="B36" s="14" t="s">
+    </row>
+    <row r="38" spans="2:12" ht="17" customHeight="1">
+      <c r="B38" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C38" s="17">
         <v>1E-4</v>
       </c>
-      <c r="D36" s="16">
+      <c r="D38" s="16">
         <v>1776481</v>
       </c>
-      <c r="E36" s="9">
-        <f t="shared" ref="E36:E44" si="0">D36*C36</f>
+      <c r="E38" s="9">
+        <f t="shared" ref="E38:E46" si="0">D38*C38</f>
         <v>177.6481</v>
       </c>
-      <c r="F36" s="12">
-        <f t="shared" ref="F36:F45" si="1">E36/D36</f>
+      <c r="F38" s="12">
+        <f t="shared" ref="F38:F47" si="1">E38/D38</f>
         <v>1E-4</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="17">
+      <c r="I38" s="17">
         <v>1E-4</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J38" s="15">
         <v>1776481</v>
       </c>
-      <c r="K36" s="9">
-        <f t="shared" ref="K36:K44" si="2">J36*I36</f>
+      <c r="K38" s="9">
+        <f t="shared" ref="K38:K46" si="2">J38*I38</f>
         <v>177.6481</v>
       </c>
-      <c r="L36" s="45">
-        <f t="shared" ref="L36:L43" si="3">IF(J36&gt;0, K36/J36,"-")</f>
+      <c r="L38" s="45">
+        <f t="shared" ref="L38:L45" si="3">IF(J38&gt;0, K38/J38,"-")</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="17" customHeight="1">
-      <c r="B37" s="14" t="s">
+    <row r="39" spans="2:12" ht="17" customHeight="1">
+      <c r="B39" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C39" s="17">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="D37" s="16">
+      <c r="D39" s="16">
         <v>2001656</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E39" s="9">
         <f t="shared" si="0"/>
         <v>400.33120000000002</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F39" s="12">
         <f t="shared" si="1"/>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="18" t="s">
+      <c r="G39" s="11"/>
+      <c r="H39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I39" s="17">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J39" s="15">
         <v>2001656</v>
       </c>
-      <c r="K37" s="9">
+      <c r="K39" s="9">
         <f t="shared" si="2"/>
         <v>400.33120000000002</v>
       </c>
-      <c r="L37" s="45">
+      <c r="L39" s="45">
         <f t="shared" si="3"/>
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="17" customHeight="1">
-      <c r="B38" s="14" t="s">
+    <row r="40" spans="2:12" ht="17" customHeight="1">
+      <c r="B40" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C40" s="17">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="D38" s="16">
+      <c r="D40" s="16">
         <v>2244283</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E40" s="9">
         <f t="shared" si="0"/>
         <v>2019.8546999999999</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F40" s="12">
         <f t="shared" si="1"/>
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="1" t="s">
+      <c r="G40" s="11"/>
+      <c r="H40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I38" s="17">
+      <c r="I40" s="17">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="J38" s="15">
+      <c r="J40" s="15">
         <v>2244283</v>
       </c>
-      <c r="K38" s="9">
+      <c r="K40" s="9">
         <f t="shared" si="2"/>
         <v>2019.8546999999999</v>
       </c>
-      <c r="L38" s="45">
+      <c r="L40" s="45">
         <f t="shared" si="3"/>
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="17" customHeight="1">
-      <c r="B39" s="14" t="s">
+    <row r="41" spans="2:12" ht="17" customHeight="1">
+      <c r="B41" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C41" s="10">
         <v>1.8E-3</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D41" s="16">
         <v>2143651</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E41" s="9">
         <f t="shared" si="0"/>
         <v>3858.5717999999997</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F41" s="12">
         <f t="shared" si="1"/>
         <v>1.8E-3</v>
       </c>
-      <c r="G39" s="131" t="s">
+      <c r="G41" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I39" s="10">
+      <c r="I41" s="10">
         <v>1.8E-3</v>
       </c>
-      <c r="J39" s="15">
+      <c r="J41" s="15">
         <v>2143651</v>
       </c>
-      <c r="K39" s="9">
+      <c r="K41" s="9">
         <f t="shared" si="2"/>
         <v>3858.5717999999997</v>
       </c>
-      <c r="L39" s="45">
+      <c r="L41" s="45">
         <f t="shared" si="3"/>
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="17" customHeight="1">
-      <c r="B40" s="14" t="s">
+    <row r="42" spans="2:12" ht="17" customHeight="1">
+      <c r="B42" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C42" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D40" s="16">
+      <c r="D42" s="16">
         <v>2206346</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E42" s="9">
         <f t="shared" si="0"/>
         <v>8825.384</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F42" s="12">
         <f t="shared" si="1"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G40" s="131"/>
-      <c r="H40" s="1" t="s">
+      <c r="G42" s="131"/>
+      <c r="H42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I40" s="10">
+      <c r="I42" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J42" s="15">
         <v>2206346</v>
       </c>
-      <c r="K40" s="9">
+      <c r="K42" s="9">
         <f t="shared" si="2"/>
         <v>8825.384</v>
       </c>
-      <c r="L40" s="45">
+      <c r="L42" s="45">
         <f t="shared" si="3"/>
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="17" customHeight="1">
-      <c r="B41" s="14" t="s">
+    <row r="43" spans="2:12" ht="17" customHeight="1">
+      <c r="B43" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C43" s="10">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D41" s="16">
+      <c r="D43" s="16">
         <v>2531817</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E43" s="9">
         <f t="shared" si="0"/>
         <v>32913.620999999999</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F43" s="12">
         <f t="shared" si="1"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G41" s="131"/>
-      <c r="H41" s="1" t="s">
+      <c r="G43" s="131"/>
+      <c r="H43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I43" s="10">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="J41" s="15">
+      <c r="J43" s="15">
         <v>84681</v>
       </c>
-      <c r="K41" s="9">
+      <c r="K43" s="9">
         <f t="shared" si="2"/>
         <v>1100.8529999999998</v>
       </c>
-      <c r="L41" s="45">
+      <c r="L43" s="45">
         <f t="shared" si="3"/>
         <v>1.2999999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="17" customHeight="1">
-      <c r="B42" s="14" t="s">
+    <row r="44" spans="2:12" ht="17" customHeight="1">
+      <c r="B44" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C44" s="10">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D42" s="16">
+      <c r="D44" s="16">
         <v>2114090</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E44" s="9">
         <f t="shared" si="0"/>
         <v>97248.14</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F44" s="12">
         <f t="shared" si="1"/>
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I42" s="10">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="J42" s="15">
-        <v>0</v>
-      </c>
-      <c r="K42" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="45" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" ht="17" customHeight="1">
-      <c r="B43" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="10">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="D43" s="16">
-        <v>1574580</v>
-      </c>
-      <c r="E43" s="9">
-        <f t="shared" si="0"/>
-        <v>154308.84</v>
-      </c>
-      <c r="F43" s="12">
-        <f t="shared" si="1"/>
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I43" s="10">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="J43" s="15">
-        <v>0</v>
-      </c>
-      <c r="K43" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="45" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="17" customHeight="1">
-      <c r="B44" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0.18</v>
-      </c>
-      <c r="D44" s="13">
-        <f>691995+129700</f>
-        <v>821695</v>
-      </c>
-      <c r="E44" s="9">
-        <f t="shared" si="0"/>
-        <v>147905.1</v>
-      </c>
-      <c r="F44" s="12">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
-      </c>
       <c r="G44" s="11"/>
       <c r="H44" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I44" s="10">
-        <v>0.18</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="J44" s="15">
         <v>0</v>
@@ -6184,126 +6339,202 @@
         <v>0</v>
       </c>
       <c r="L44" s="45" t="str">
-        <f>IF(J44&gt;0, K44/J44,"-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="17" customHeight="1">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="D45" s="16">
+        <v>1574580</v>
+      </c>
+      <c r="E45" s="9">
+        <f t="shared" si="0"/>
+        <v>154308.84</v>
+      </c>
+      <c r="F45" s="12">
+        <f t="shared" si="1"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45" s="10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J45" s="15">
+        <v>0</v>
+      </c>
+      <c r="K45" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="17" customHeight="1">
+      <c r="B46" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="D46" s="13">
+        <f>691995+129700</f>
+        <v>821695</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" si="0"/>
+        <v>147905.1</v>
+      </c>
+      <c r="F46" s="12">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="G46" s="11"/>
+      <c r="H46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="J46" s="15">
+        <v>0</v>
+      </c>
+      <c r="K46" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="45" t="str">
+        <f>IF(J46&gt;0, K46/J46,"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="17" customHeight="1">
+      <c r="B47" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C45" s="40"/>
-      <c r="D45" s="8">
-        <f>SUM(D36:D44)</f>
+      <c r="C47" s="40"/>
+      <c r="D47" s="8">
+        <f>SUM(D38:D46)</f>
         <v>17414599</v>
       </c>
-      <c r="E45" s="6">
-        <f>SUM(E36:E44)</f>
+      <c r="E47" s="6">
+        <f>SUM(E38:E46)</f>
         <v>447657.49080000003</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F47" s="5">
         <f t="shared" si="1"/>
         <v>2.5705874180622822E-2</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="39">
-        <f>SUM(J36:J44)</f>
+      <c r="I47" s="40"/>
+      <c r="J47" s="39">
+        <f>SUM(J38:J46)</f>
         <v>10457098</v>
       </c>
-      <c r="K45" s="6">
-        <f>SUM(K36:K44)</f>
+      <c r="K47" s="6">
+        <f>SUM(K38:K46)</f>
         <v>16382.642799999998</v>
       </c>
-      <c r="L45" s="48">
-        <f>K45/J45</f>
+      <c r="L47" s="48">
+        <f>K47/J47</f>
         <v>1.5666528897405377E-3</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="17" customHeight="1"/>
-    <row r="47" spans="2:12" ht="17" customHeight="1"/>
-    <row r="48" spans="2:12" ht="17" customHeight="1">
-      <c r="B48" s="23" t="s">
+    <row r="48" spans="2:12" ht="17" customHeight="1"/>
+    <row r="49" spans="2:3" ht="17" customHeight="1"/>
+    <row r="50" spans="2:3" ht="17" customHeight="1">
+      <c r="B50" s="23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="17" customHeight="1">
-      <c r="B49" s="1" t="s">
+    <row r="51" spans="2:3" ht="17" customHeight="1">
+      <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="17" customHeight="1"/>
-    <row r="51" spans="2:3" ht="17" customHeight="1">
-      <c r="B51" s="49">
-        <f>L45</f>
+    <row r="52" spans="2:3" ht="17" customHeight="1"/>
+    <row r="53" spans="2:3" ht="17" customHeight="1">
+      <c r="B53" s="49">
+        <f>L47</f>
         <v>1.5666528897405377E-3</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="17" customHeight="1">
-      <c r="B52" s="3">
-        <f>F45</f>
+    <row r="54" spans="2:3" ht="17" customHeight="1">
+      <c r="B54" s="3">
+        <f>F47</f>
         <v>2.5705874180622822E-2</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="17" customHeight="1">
-      <c r="B53" s="2">
-        <f>L45/F45</f>
+    <row r="55" spans="2:3" ht="17" customHeight="1">
+      <c r="B55" s="2">
+        <f>L47/F47</f>
         <v>6.0945326299056038E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="17" customHeight="1"/>
-    <row r="55" spans="2:3" ht="17" customHeight="1">
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="2:3" ht="17" customHeight="1"/>
+    <row r="57" spans="2:3" ht="17" customHeight="1">
+      <c r="B57" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="17" customHeight="1">
-      <c r="B56" s="1" t="s">
+    <row r="58" spans="2:3" ht="17" customHeight="1">
+      <c r="B58" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="G41:G43"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="J45">
+  <conditionalFormatting sqref="J47">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="between">
-      <formula>$D$9-0.5</formula>
-      <formula>$D$9+0.5</formula>
+      <formula>$D$11-0.5</formula>
+      <formula>$D$11+0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
-      <formula>$B$53</formula>
+      <formula>$B$55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="D27">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>$L$45</formula>
+      <formula>$L$47</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1"/>
-    <hyperlink ref="G8" r:id="rId2"/>
-    <hyperlink ref="G18" r:id="rId3"/>
-    <hyperlink ref="G19" r:id="rId4"/>
-    <hyperlink ref="N13" r:id="rId5"/>
-    <hyperlink ref="K12" r:id="rId6"/>
-    <hyperlink ref="C31" r:id="rId7"/>
-    <hyperlink ref="C32" r:id="rId8" location="/CBS/nl/dataset/84646NED/table?ts=1584394178496"/>
-    <hyperlink ref="K13" r:id="rId9"/>
+    <hyperlink ref="G9" r:id="rId1"/>
+    <hyperlink ref="G10" r:id="rId2"/>
+    <hyperlink ref="G20" r:id="rId3"/>
+    <hyperlink ref="G21" r:id="rId4"/>
+    <hyperlink ref="P15" r:id="rId5"/>
+    <hyperlink ref="L14" r:id="rId6"/>
+    <hyperlink ref="C33" r:id="rId7"/>
+    <hyperlink ref="C34" r:id="rId8" location="/CBS/nl/dataset/84646NED/table?ts=1584394178496"/>
+    <hyperlink ref="M15" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -6324,7 +6555,7 @@
               <x14:cfIcon iconSet="3Stars" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>J36:J40 D18:D19 D12:D14 D7:D8</xm:sqref>
+          <xm:sqref>J38:J42 D20:D21 D14:D16 D9:D10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="13" id="{A57E04D3-B3C6-F845-B835-4222379C636D}">
@@ -6343,7 +6574,7 @@
               <x14:cfIcon iconSet="3Stars" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>D25</xm:sqref>
+          <xm:sqref>D27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="1" id="{DCF96E41-D9C5-B840-BE3D-711AEED74DE6}">
@@ -6362,7 +6593,7 @@
               <x14:cfIcon iconSet="3Stars" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>J41:J44</xm:sqref>
+          <xm:sqref>J43:J46</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6378,7 +6609,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6400,7 +6631,7 @@
       <c r="Q1"/>
       <c r="R1"/>
       <c r="T1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:21">
@@ -6444,10 +6675,12 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="51"/>
-      <c r="L5"/>
+      <c r="L5" t="s">
+        <v>146</v>
+      </c>
       <c r="M5"/>
       <c r="O5"/>
       <c r="P5"/>
@@ -6471,13 +6704,13 @@
         <v>45</v>
       </c>
       <c r="D6" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="58" t="s">
         <v>139</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>138</v>
-      </c>
-      <c r="F6" s="58" t="s">
-        <v>140</v>
       </c>
       <c r="G6" s="58" t="s">
         <v>86</v>
@@ -6491,9 +6724,18 @@
       <c r="J6" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="O6"/>
+      <c r="L6" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="M6" t="s">
+        <v>143</v>
+      </c>
+      <c r="N6" t="s">
+        <v>144</v>
+      </c>
+      <c r="O6" t="s">
+        <v>148</v>
+      </c>
       <c r="P6"/>
       <c r="Q6"/>
       <c r="R6"/>
@@ -6540,9 +6782,19 @@
         <f t="shared" ref="J7:J15" si="2">AVERAGE(F7:G7)</f>
         <v>0.48749999999999999</v>
       </c>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="O7"/>
+      <c r="L7" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>21</v>
+      </c>
+      <c r="N7">
+        <v>43668</v>
+      </c>
+      <c r="O7" s="60">
+        <f>M7/N7</f>
+        <v>4.8090134652377029E-4</v>
+      </c>
       <c r="P7"/>
       <c r="Q7"/>
       <c r="R7"/>
@@ -6589,9 +6841,19 @@
         <f t="shared" si="2"/>
         <v>0.453056075</v>
       </c>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="O8"/>
+      <c r="L8" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8">
+        <v>76</v>
+      </c>
+      <c r="N8">
+        <v>44269</v>
+      </c>
+      <c r="O8" s="60">
+        <f t="shared" ref="O8:O16" si="5">M8/N8</f>
+        <v>1.7167769771171701E-3</v>
+      </c>
       <c r="P8"/>
       <c r="Q8"/>
       <c r="R8"/>
@@ -6638,9 +6900,19 @@
         <f t="shared" si="2"/>
         <v>0.84753524999999996</v>
       </c>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="O9"/>
+      <c r="L9" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>158</v>
+      </c>
+      <c r="N9">
+        <v>48238</v>
+      </c>
+      <c r="O9" s="60">
+        <f t="shared" si="5"/>
+        <v>3.2754260126870932E-3</v>
+      </c>
       <c r="P9"/>
       <c r="Q9"/>
       <c r="R9"/>
@@ -6687,9 +6959,19 @@
         <f t="shared" si="2"/>
         <v>0.76700049999999997</v>
       </c>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="O10"/>
+      <c r="L10" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>171</v>
+      </c>
+      <c r="N10">
+        <v>46464</v>
+      </c>
+      <c r="O10" s="60">
+        <f t="shared" si="5"/>
+        <v>3.6802685950413222E-3</v>
+      </c>
       <c r="P10"/>
       <c r="Q10"/>
       <c r="R10"/>
@@ -6736,9 +7018,19 @@
         <f t="shared" si="2"/>
         <v>0.68032985000000001</v>
       </c>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="O11"/>
+      <c r="L11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11">
+        <v>226</v>
+      </c>
+      <c r="N11">
+        <v>42622</v>
+      </c>
+      <c r="O11" s="60">
+        <f t="shared" si="5"/>
+        <v>5.3024259771948757E-3</v>
+      </c>
       <c r="P11"/>
       <c r="Q11"/>
       <c r="R11"/>
@@ -6785,9 +7077,19 @@
         <f t="shared" si="2"/>
         <v>0.47589535000000005</v>
       </c>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="O12"/>
+      <c r="L12" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>190</v>
+      </c>
+      <c r="N12">
+        <v>42276</v>
+      </c>
+      <c r="O12" s="60">
+        <f t="shared" si="5"/>
+        <v>4.4942757119878895E-3</v>
+      </c>
       <c r="P12"/>
       <c r="Q12"/>
       <c r="R12"/>
@@ -6834,9 +7136,19 @@
         <f t="shared" si="2"/>
         <v>0.4305814</v>
       </c>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="O13"/>
+      <c r="L13" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>131</v>
+      </c>
+      <c r="N13">
+        <v>36635</v>
+      </c>
+      <c r="O13" s="60">
+        <f t="shared" si="5"/>
+        <v>3.575815477002866E-3</v>
+      </c>
       <c r="P13"/>
       <c r="Q13"/>
       <c r="R13"/>
@@ -6883,9 +7195,19 @@
         <f t="shared" si="2"/>
         <v>0.40718965000000001</v>
       </c>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="O14"/>
+      <c r="L14" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>37</v>
+      </c>
+      <c r="N14">
+        <v>22223</v>
+      </c>
+      <c r="O14" s="60">
+        <f t="shared" si="5"/>
+        <v>1.6649417270395536E-3</v>
+      </c>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
@@ -6926,18 +7248,38 @@
         <f t="shared" si="2"/>
         <v>0.53493520000000006</v>
       </c>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="O15"/>
+      <c r="L15" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>10258</v>
+      </c>
+      <c r="O15" s="60">
+        <f t="shared" si="5"/>
+        <v>3.8993955936829789E-4</v>
+      </c>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="50"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="O16"/>
+      <c r="L16" s="50" t="s">
+        <v>147</v>
+      </c>
+      <c r="M16">
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>2384</v>
+      </c>
+      <c r="O16" s="60">
+        <f t="shared" si="5"/>
+        <v>2.5167785234899327E-3</v>
+      </c>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>

</xml_diff>